<commit_message>
Port Number for Communication with Ground
</commit_message>
<xml_diff>
--- a/Spaceship/LogFiles.xlsx
+++ b/Spaceship/LogFiles.xlsx
@@ -339,6 +339,12 @@
   <x:si>
     <x:t>9.943185</x:t>
   </x:si>
+  <x:si>
+    <x:t>2024 November 26 5:20:00 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>X:999.44, Y:1999.65, Z:2999.14</x:t>
+  </x:si>
 </x:sst>
 </file>
 
@@ -849,6 +855,12 @@
         <x:v>109</x:v>
       </x:c>
     </x:row>
+    <x:row r="37">
+      <x:c r="A37"/>
+      <x:c r="B37"/>
+      <x:c r="C37"/>
+      <x:c r="D37"/>
+    </x:row>
   </x:sheetData>
 </x:worksheet>
 </file>
</xml_diff>